<commit_message>
move py file to py_files
</commit_message>
<xml_diff>
--- a/first_wb.xlsx
+++ b/first_wb.xlsx
@@ -83,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -101,6 +101,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" indent="2"/>
@@ -610,7 +613,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>It is a long established fact that a reader will be distracted by thereadable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English. Many desktop publishing packages and web page editors now use Lorem Ipsum as their default model text, and a search for 'lorem ipsum' will uncover many web sites still in their infancy. Various versions have evolved over the years, sometimes by accident, sometimes on purpose (injected humour and the like).</t>
         </is>

</xml_diff>

<commit_message>
add border and background style
</commit_message>
<xml_diff>
--- a/first_wb.xlsx
+++ b/first_wb.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -44,8 +44,12 @@
       <sz val="24"/>
       <u val="double"/>
     </font>
+    <font>
+      <name val="Berlin Sans FB Demi"/>
+      <color rgb="00FDF7E4"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -55,8 +59,20 @@
     <fill>
       <patternFill patternType="solid"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEE2DE"/>
+        <bgColor rgb="FF2B2A4C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B31312"/>
+        <bgColor rgb="006B240C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -79,11 +95,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color rgb="FF2B2A4C"/>
+      </right>
+      <top style="dashDotDot">
+        <color rgb="FF265073"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF6B240C"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -92,22 +123,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,10 +605,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="25.53125" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="25.53125" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30.75" customHeight="1" s="4">
+    <row r="1" ht="30.75" customHeight="1" s="7">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Font Testing</t>
@@ -604,18 +626,45 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="23.46484375" customWidth="1" style="7" min="1" max="1"/>
+    <col width="16.59765625" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="16.59765625" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
+    <col width="17.265625" bestFit="1" customWidth="1" style="7" min="10" max="10"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>It is a long established fact that a reader will be distracted by thereadable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English. Many desktop publishing packages and web page editors now use Lorem Ipsum as their default model text, and a search for 'lorem ipsum' will uncover many web sites still in their infancy. Various versions have evolved over the years, sometimes by accident, sometimes on purpose (injected humour and the like).</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Visual Studio Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="H5" s="6" t="inlineStr">
+        <is>
+          <t>Background Style</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>Background Style 2</t>
         </is>
       </c>
     </row>
@@ -685,7 +734,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="20" customWidth="1" style="4" min="1" max="28"/>
+    <col width="20" customWidth="1" style="7" min="1" max="28"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
add chart and conditional case
</commit_message>
<xml_diff>
--- a/first_wb.xlsx
+++ b/first_wb.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\python-openpyxl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECF9FB3-91CC-42AE-8C93-B1047033BB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545B97F-B0C2-4F79-B241-D97C8F136412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="6930" windowWidth="38640" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="6930" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="First" sheetId="2" r:id="rId2"/>
     <sheet name="Fonts" sheetId="3" r:id="rId3"/>
     <sheet name="Text_Alignment" sheetId="4" r:id="rId4"/>
-    <sheet name="Second" sheetId="5" r:id="rId5"/>
+    <sheet name="Conditional" sheetId="5" r:id="rId5"/>
     <sheet name="Third" sheetId="6" r:id="rId6"/>
     <sheet name="LTE_CIQ" sheetId="7" r:id="rId7"/>
     <sheet name="family_data" sheetId="8" r:id="rId8"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="203">
   <si>
     <t>Font Testing</t>
   </si>
@@ -44,7 +44,19 @@
     <t>Background Style 2</t>
   </si>
   <si>
-    <t>Merge Cells</t>
+    <t>rand1</t>
+  </si>
+  <si>
+    <t>rand2</t>
+  </si>
+  <si>
+    <t>rand3</t>
+  </si>
+  <si>
+    <t>rand4</t>
+  </si>
+  <si>
+    <t>rand5</t>
   </si>
   <si>
     <t>GSM_Common_ID</t>
@@ -658,7 +670,7 @@
       <name val="Berlin Sans FB Demi"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,6 +690,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB31312"/>
         <bgColor rgb="FF6B240C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF96EFFF"/>
+        <bgColor rgb="FFC5FFF8"/>
       </patternFill>
     </fill>
   </fills>
@@ -738,7 +756,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,6 +772,949 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Family Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>family_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>age</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>family_data!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>endang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>indah</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>alde</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>aqeela</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>auza</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>arsyila</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>akhdan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>family_data!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9514-475B-BEDE-E4AE9C9CB221}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="10"/>
+        <c:axId val="100"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ID"/>
+                  <a:t>Name</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ID"/>
+                  <a:t>Age</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Family Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>family_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>age</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>family_data!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>endang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>indah</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>alde</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>aqeela</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>auza</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>arsyila</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>akhdan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>family_data!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-811D-41DC-A44B-B9C4A91A2B6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="10"/>
+        <c:axId val="100"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ID"/>
+                  <a:t>Name</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ID"/>
+                  <a:t>Age</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Family Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>family_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>age</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>family_data!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>endang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>indah</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>alde</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>aqeela</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>auza</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>arsyila</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>akhdan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>family_data!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7596-416B-990D-1D6BF617E35F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="10"/>
+        <c:axId val="100"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Family Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>family_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>age</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>family_data!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>endang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>indah</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>alde</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>aqeela</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>auza</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>arsyila</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>akhdan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>family_data!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1FAA-488A-8BFB-BFA294CE8D22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="10"/>
+        <c:axId val="100"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Family Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>family_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>age</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7188-456D-891B-156D905BFAF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="10"/>
+        <c:axId val="20"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="20"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="20"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -828,6 +1789,166 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -1209,26 +2330,882 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="E1:J1"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>959</v>
+      </c>
+      <c r="B2">
+        <v>739</v>
+      </c>
+      <c r="C2">
+        <v>580</v>
+      </c>
+      <c r="D2">
+        <v>799</v>
+      </c>
+      <c r="E2">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>878</v>
+      </c>
+      <c r="B3">
+        <v>865</v>
+      </c>
+      <c r="C3">
+        <v>610</v>
+      </c>
+      <c r="D3">
+        <v>892</v>
+      </c>
+      <c r="E3">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>283</v>
+      </c>
+      <c r="B4">
+        <v>131</v>
+      </c>
+      <c r="C4">
+        <v>970</v>
+      </c>
+      <c r="D4">
+        <v>435</v>
+      </c>
+      <c r="E4">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>484</v>
+      </c>
+      <c r="B5">
+        <v>548</v>
+      </c>
+      <c r="C5">
+        <v>991</v>
+      </c>
+      <c r="D5">
+        <v>693</v>
+      </c>
+      <c r="E5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>674</v>
+      </c>
+      <c r="B6">
+        <v>445</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>258</v>
+      </c>
+      <c r="E6">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>344</v>
+      </c>
+      <c r="B7" s="8">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>134</v>
+      </c>
+      <c r="D7">
+        <v>681</v>
+      </c>
+      <c r="E7">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>866</v>
+      </c>
+      <c r="B8">
+        <v>268</v>
+      </c>
+      <c r="C8">
+        <v>860</v>
+      </c>
+      <c r="D8">
+        <v>536</v>
+      </c>
+      <c r="E8">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="8">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>242</v>
+      </c>
+      <c r="C9">
+        <v>420</v>
+      </c>
+      <c r="D9">
+        <v>703</v>
+      </c>
+      <c r="E9">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>811</v>
+      </c>
+      <c r="B10" s="8">
+        <v>73</v>
+      </c>
+      <c r="C10">
+        <v>260</v>
+      </c>
+      <c r="D10">
+        <v>355</v>
+      </c>
+      <c r="E10" s="8">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>281</v>
+      </c>
+      <c r="B11">
+        <v>502</v>
+      </c>
+      <c r="C11">
+        <v>948</v>
+      </c>
+      <c r="D11">
+        <v>534</v>
+      </c>
+      <c r="E11">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>218</v>
+      </c>
+      <c r="B12">
+        <v>975</v>
+      </c>
+      <c r="C12">
+        <v>819</v>
+      </c>
+      <c r="D12">
+        <v>612</v>
+      </c>
+      <c r="E12">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>860</v>
+      </c>
+      <c r="B13">
+        <v>631</v>
+      </c>
+      <c r="C13">
+        <v>334</v>
+      </c>
+      <c r="D13">
+        <v>440</v>
+      </c>
+      <c r="E13">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>739</v>
+      </c>
+      <c r="B14">
+        <v>133</v>
+      </c>
+      <c r="C14">
+        <v>602</v>
+      </c>
+      <c r="D14">
+        <v>587</v>
+      </c>
+      <c r="E14">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>764</v>
+      </c>
+      <c r="B15">
+        <v>392</v>
+      </c>
+      <c r="C15">
+        <v>428</v>
+      </c>
+      <c r="D15">
+        <v>472</v>
+      </c>
+      <c r="E15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>533</v>
+      </c>
+      <c r="B16">
+        <v>416</v>
+      </c>
+      <c r="C16" s="8">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>628</v>
+      </c>
+      <c r="E16">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>509</v>
+      </c>
+      <c r="B17">
+        <v>881</v>
+      </c>
+      <c r="C17">
+        <v>762</v>
+      </c>
+      <c r="D17">
+        <v>878</v>
+      </c>
+      <c r="E17">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>569</v>
+      </c>
+      <c r="B18">
+        <v>466</v>
+      </c>
+      <c r="C18">
+        <v>968</v>
+      </c>
+      <c r="D18" s="8">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>279</v>
+      </c>
+      <c r="B19">
+        <v>360</v>
+      </c>
+      <c r="C19">
+        <v>713</v>
+      </c>
+      <c r="D19">
+        <v>615</v>
+      </c>
+      <c r="E19">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>906</v>
+      </c>
+      <c r="B20">
+        <v>182</v>
+      </c>
+      <c r="C20">
+        <v>943</v>
+      </c>
+      <c r="D20">
+        <v>930</v>
+      </c>
+      <c r="E20">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>736</v>
+      </c>
+      <c r="B21">
+        <v>379</v>
+      </c>
+      <c r="C21">
+        <v>441</v>
+      </c>
+      <c r="D21">
+        <v>498</v>
+      </c>
+      <c r="E21">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>842</v>
+      </c>
+      <c r="B22">
+        <v>551</v>
+      </c>
+      <c r="C22">
+        <v>900</v>
+      </c>
+      <c r="D22">
+        <v>630</v>
+      </c>
+      <c r="E22">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>594</v>
+      </c>
+      <c r="B23">
+        <v>318</v>
+      </c>
+      <c r="C23">
+        <v>647</v>
+      </c>
+      <c r="D23">
+        <v>254</v>
+      </c>
+      <c r="E23">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>122</v>
+      </c>
+      <c r="B24">
+        <v>117</v>
+      </c>
+      <c r="C24">
+        <v>811</v>
+      </c>
+      <c r="D24">
+        <v>224</v>
+      </c>
+      <c r="E24">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>502</v>
+      </c>
+      <c r="B25">
+        <v>907</v>
+      </c>
+      <c r="C25">
+        <v>737</v>
+      </c>
+      <c r="D25">
+        <v>525</v>
+      </c>
+      <c r="E25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>713</v>
+      </c>
+      <c r="B26">
+        <v>991</v>
+      </c>
+      <c r="C26">
+        <v>929</v>
+      </c>
+      <c r="D26" s="8">
+        <v>68</v>
+      </c>
+      <c r="E26">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>604</v>
+      </c>
+      <c r="B27">
+        <v>612</v>
+      </c>
+      <c r="C27" s="8">
+        <v>90</v>
+      </c>
+      <c r="D27">
+        <v>816</v>
+      </c>
+      <c r="E27">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>555</v>
+      </c>
+      <c r="B28">
+        <v>489</v>
+      </c>
+      <c r="C28">
+        <v>270</v>
+      </c>
+      <c r="D28" s="8">
+        <v>91</v>
+      </c>
+      <c r="E28">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>442</v>
+      </c>
+      <c r="B29" s="8">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>406</v>
+      </c>
+      <c r="D29">
+        <v>904</v>
+      </c>
+      <c r="E29">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>463</v>
+      </c>
+      <c r="B30">
+        <v>609</v>
+      </c>
+      <c r="C30">
+        <v>728</v>
+      </c>
+      <c r="D30">
+        <v>143</v>
+      </c>
+      <c r="E30">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>983</v>
+      </c>
+      <c r="B31">
+        <v>644</v>
+      </c>
+      <c r="C31">
+        <v>905</v>
+      </c>
+      <c r="D31">
+        <v>888</v>
+      </c>
+      <c r="E31">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>363</v>
+      </c>
+      <c r="B32">
+        <v>779</v>
+      </c>
+      <c r="C32">
+        <v>487</v>
+      </c>
+      <c r="D32" s="8">
+        <v>67</v>
+      </c>
+      <c r="E32">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>149</v>
+      </c>
+      <c r="B33">
+        <v>868</v>
+      </c>
+      <c r="C33">
+        <v>697</v>
+      </c>
+      <c r="D33">
+        <v>410</v>
+      </c>
+      <c r="E33">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>436</v>
+      </c>
+      <c r="B34">
+        <v>900</v>
+      </c>
+      <c r="C34">
+        <v>640</v>
+      </c>
+      <c r="D34">
+        <v>405</v>
+      </c>
+      <c r="E34">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>827</v>
+      </c>
+      <c r="B35">
+        <v>140</v>
+      </c>
+      <c r="C35">
+        <v>866</v>
+      </c>
+      <c r="D35" s="8">
+        <v>25</v>
+      </c>
+      <c r="E35">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>659</v>
+      </c>
+      <c r="B36">
+        <v>466</v>
+      </c>
+      <c r="C36">
+        <v>528</v>
+      </c>
+      <c r="D36">
+        <v>894</v>
+      </c>
+      <c r="E36">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>228</v>
+      </c>
+      <c r="B37">
+        <v>249</v>
+      </c>
+      <c r="C37">
+        <v>542</v>
+      </c>
+      <c r="D37">
+        <v>729</v>
+      </c>
+      <c r="E37" s="8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>289</v>
+      </c>
+      <c r="B38">
+        <v>363</v>
+      </c>
+      <c r="C38">
+        <v>436</v>
+      </c>
+      <c r="D38">
+        <v>295</v>
+      </c>
+      <c r="E38">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>634</v>
+      </c>
+      <c r="B39">
+        <v>650</v>
+      </c>
+      <c r="C39">
+        <v>280</v>
+      </c>
+      <c r="D39">
+        <v>426</v>
+      </c>
+      <c r="E39">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>172</v>
+      </c>
+      <c r="B40">
+        <v>550</v>
+      </c>
+      <c r="C40">
+        <v>915</v>
+      </c>
+      <c r="D40">
+        <v>149</v>
+      </c>
+      <c r="E40">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>966</v>
+      </c>
+      <c r="B41">
+        <v>216</v>
+      </c>
+      <c r="C41">
+        <v>341</v>
+      </c>
+      <c r="D41">
+        <v>442</v>
+      </c>
+      <c r="E41">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>529</v>
+      </c>
+      <c r="B42">
+        <v>632</v>
+      </c>
+      <c r="C42">
+        <v>280</v>
+      </c>
+      <c r="D42">
+        <v>385</v>
+      </c>
+      <c r="E42">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>808</v>
+      </c>
+      <c r="B43">
+        <v>227</v>
+      </c>
+      <c r="C43">
+        <v>915</v>
+      </c>
+      <c r="D43">
+        <v>862</v>
+      </c>
+      <c r="E43">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>678</v>
+      </c>
+      <c r="B44" s="8">
+        <v>70</v>
+      </c>
+      <c r="C44">
+        <v>656</v>
+      </c>
+      <c r="D44">
+        <v>627</v>
+      </c>
+      <c r="E44">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>175</v>
+      </c>
+      <c r="B45">
+        <v>305</v>
+      </c>
+      <c r="C45" s="8">
+        <v>21</v>
+      </c>
+      <c r="D45">
+        <v>223</v>
+      </c>
+      <c r="E45">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>227</v>
+      </c>
+      <c r="B46">
+        <v>529</v>
+      </c>
+      <c r="C46">
+        <v>735</v>
+      </c>
+      <c r="D46">
+        <v>541</v>
+      </c>
+      <c r="E46">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>711</v>
+      </c>
+      <c r="B47">
+        <v>952</v>
+      </c>
+      <c r="C47" s="8">
+        <v>90</v>
+      </c>
+      <c r="D47">
+        <v>769</v>
+      </c>
+      <c r="E47">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>868</v>
+      </c>
+      <c r="B48">
+        <v>547</v>
+      </c>
+      <c r="C48">
+        <v>438</v>
+      </c>
+      <c r="D48">
+        <v>599</v>
+      </c>
+      <c r="E48">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>302</v>
+      </c>
+      <c r="B49">
+        <v>766</v>
+      </c>
+      <c r="C49">
+        <v>786</v>
+      </c>
+      <c r="D49">
+        <v>427</v>
+      </c>
+      <c r="E49">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>174</v>
+      </c>
+      <c r="B50">
+        <v>272</v>
+      </c>
+      <c r="C50">
+        <v>909</v>
+      </c>
+      <c r="D50">
+        <v>596</v>
+      </c>
+      <c r="E50">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>358</v>
+      </c>
+      <c r="B51">
+        <v>123</v>
+      </c>
+      <c r="C51">
+        <v>582</v>
+      </c>
+      <c r="D51">
+        <v>702</v>
+      </c>
+      <c r="E51">
+        <v>479</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:J1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1260,1636 +3237,1636 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="AA3" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="P4" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="V6" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="Q7" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="V9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="Y9" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="Q10" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="U12" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="V12" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N13" s="2" t="s">
+      <c r="S13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="V13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="W13" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="U15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="V15" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T18" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="V18" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="Q19" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2901,8 +4878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2912,27 +4889,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B2">
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F2">
         <v>113</v>
@@ -2940,16 +4917,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B3">
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F3">
         <v>16.142857142857139</v>
@@ -2957,60 +4934,61 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B4">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B5">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>